<commit_message>
Base data which Alex and Lukas have already analysed
</commit_message>
<xml_diff>
--- a/src/output_detections_highlighting_with_annotations.xlsx
+++ b/src/output_detections_highlighting_with_annotations.xlsx
@@ -8,9 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Incomplete US labelling" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Time Consup. Anlys.S." sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incomplete US labelling'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Time Consup. Anlys.S.'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -3787,4 +3789,587 @@
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.5" customWidth="1" min="1" max="1"/>
+    <col width="16.5" customWidth="1" min="2" max="2"/>
+    <col width="22.5" customWidth="1" min="3" max="3"/>
+    <col width="28.5" customWidth="1" min="4" max="4"/>
+    <col width="19.5" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="13.5" customWidth="1" min="7" max="7"/>
+    <col width="13.5" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Run Count</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Model Version</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Threading Enabled</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Nanoseconds</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Milliseconds</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Seconds</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Minutes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>g03</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>24432056000</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>24432.056</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>24.432056</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0.4072009333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>g04</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>19673610600</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>19673.6106</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>19.6736106</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.32789351</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>g08</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>20509298100</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>20509.2981</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>20.5092981</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.341821635</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>g10</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>19577699500</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>19577.6995</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>19.5776995</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0.3262949916666667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>g11</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>18555636500</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>18555.6365</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>18.5556365</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0.3092606083333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>g14</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>20233035800</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>20233.0358</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>20.2330358</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0.3372172633333334</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>g16</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>19085965900</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>19085.9659</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>19.0859659</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0.3180994316666667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>g18</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>24575900600</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>24575.9006</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>24.5759006</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0.4095983433333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>g19</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>19026639000</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>19026.639</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>19.026639</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.31711065</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>g21</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>19818092700</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>19818.0927</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>19.8180927</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0.330301545</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>g22</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>19700350100</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>19700.3501</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>19.7003501</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>0.3283391683333334</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>g23</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>22254455400</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>22254.4554</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>22.2544554</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>0.37090759</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>g24</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>23285504400</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>23285.5044</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>23.2855044</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>0.38809174</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>g25</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>24368524200</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>24368.5242</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>24.3685242</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>0.40614207</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>g26</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>23959839400</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>23959.8394</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>23.9598394</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>0.3993306566666667</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>g27</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>23580391800</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>23580.3918</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>23.5803918</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>0.39300653</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>g28</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>24813442900</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>24813.4429</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>24.8134429</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>0.4135573816666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>